<commit_message>
updating RTM & SIQ
</commit_message>
<xml_diff>
--- a/Managment/Requirments/ACS_RTM.xlsx
+++ b/Managment/Requirments/ACS_RTM.xlsx
@@ -13,14 +13,13 @@
   </bookViews>
   <sheets>
     <sheet name="RTM" sheetId="3" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>REQUIREMENTS TRACEABILITY MATRIX</t>
   </si>
@@ -66,9 +65,6 @@
 (System Requirments Specification)</t>
   </si>
   <si>
-    <t>Satisfied</t>
-  </si>
-  <si>
     <t>Architectural/Design
  Document</t>
   </si>
@@ -85,12 +81,6 @@
   </si>
   <si>
     <t>SIQ_5</t>
-  </si>
-  <si>
-    <t>Waiting to an answer</t>
-  </si>
-  <si>
-    <t>Unsatisfied</t>
   </si>
   <si>
     <t>2.0.3</t>
@@ -288,7 +278,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -330,7 +320,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -659,8 +648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z996"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -675,16 +664,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="12.75">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
       <c r="I1" s="1"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
@@ -705,18 +694,18 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" ht="12.75">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="27" t="s">
+      <c r="B2" s="21"/>
+      <c r="C2" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
       <c r="I2" s="1"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
@@ -736,11 +725,11 @@
       <c r="Y2" s="2"/>
       <c r="Z2" s="2"/>
     </row>
-    <row r="3" spans="1:26" s="6" customFormat="1" ht="51">
+    <row r="3" spans="1:26" s="6" customFormat="1" ht="38.25">
       <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="17" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -749,17 +738,17 @@
       <c r="D3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="17" t="s">
         <v>13</v>
       </c>
       <c r="F3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>17</v>
       </c>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
@@ -784,19 +773,19 @@
       <c r="A4" s="7">
         <v>1</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="17" t="s">
-        <v>23</v>
+      <c r="C4" s="16" t="s">
+        <v>20</v>
       </c>
-      <c r="D4" s="20" t="s">
-        <v>32</v>
+      <c r="D4" s="19" t="s">
+        <v>29</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
-      <c r="F4" s="19"/>
+      <c r="F4" s="18"/>
       <c r="G4" s="7"/>
       <c r="H4" s="8"/>
       <c r="I4" s="1"/>
@@ -819,24 +808,24 @@
       <c r="Z4" s="2"/>
     </row>
     <row r="5" spans="1:26" ht="27" customHeight="1">
-      <c r="A5" s="29">
+      <c r="A5" s="28">
         <v>2</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="23" t="s">
-        <v>18</v>
+      <c r="C5" s="22" t="s">
+        <v>17</v>
       </c>
-      <c r="D5" s="23" t="s">
-        <v>30</v>
+      <c r="D5" s="22" t="s">
+        <v>27</v>
       </c>
-      <c r="E5" s="23" t="s">
-        <v>24</v>
+      <c r="E5" s="22" t="s">
+        <v>21</v>
       </c>
-      <c r="F5" s="30"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
@@ -857,14 +846,14 @@
       <c r="Z5" s="2"/>
     </row>
     <row r="6" spans="1:26" ht="52.5" customHeight="1">
-      <c r="A6" s="29"/>
-      <c r="B6" s="28"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="29"/>
-      <c r="H6" s="29"/>
+      <c r="A6" s="28"/>
+      <c r="B6" s="27"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
@@ -892,13 +881,13 @@
         <v>5</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
-      <c r="E7" s="23"/>
-      <c r="F7" s="19"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="18"/>
       <c r="G7" s="9"/>
       <c r="H7" s="8"/>
       <c r="I7" s="2"/>
@@ -928,13 +917,13 @@
         <v>6</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
-      <c r="E8" s="23"/>
-      <c r="F8" s="19"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="18"/>
       <c r="G8" s="9"/>
       <c r="H8" s="8"/>
       <c r="I8" s="2"/>
@@ -964,13 +953,13 @@
         <v>7</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E9" s="7"/>
-      <c r="F9" s="19"/>
+      <c r="F9" s="18"/>
       <c r="G9" s="7"/>
       <c r="H9" s="8"/>
       <c r="I9" s="1"/>
@@ -1000,13 +989,13 @@
         <v>8</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E10" s="7"/>
-      <c r="F10" s="19"/>
+      <c r="F10" s="18"/>
       <c r="G10" s="7"/>
       <c r="H10" s="8"/>
       <c r="I10" s="1"/>
@@ -28657,38 +28646,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
-  <cols>
-    <col min="1" max="1" width="23.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A1" s="15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A2" s="15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A3" s="15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
updating RTM removing hyperlinks
</commit_message>
<xml_diff>
--- a/Managment/Requirments/ACS_RTM.xlsx
+++ b/Managment/Requirments/ACS_RTM.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Air-Conditioner-Screen-Team-4\Managment\Requirments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Air-Conditioner-Screen-Team-4\Managment\Requirments\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="RTM" sheetId="3" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -164,8 +164,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="12">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -224,20 +224,6 @@
       <name val="Century Gothic"/>
       <family val="2"/>
     </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Century Gothic"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color theme="4" tint="-0.499984740745262"/>
-      <name val="Century Gothic"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -278,7 +264,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -317,15 +303,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -334,6 +311,9 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -364,6 +344,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -649,7 +632,7 @@
   <dimension ref="A1:Z996"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -664,16 +647,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="12.75">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
       <c r="I1" s="1"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
@@ -694,18 +677,18 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" ht="12.75">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="26" t="s">
+      <c r="B2" s="19"/>
+      <c r="C2" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
       <c r="I2" s="1"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
@@ -729,7 +712,7 @@
       <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="14" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -738,7 +721,7 @@
       <c r="D3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="14" t="s">
         <v>13</v>
       </c>
       <c r="F3" s="4" t="s">
@@ -769,63 +752,63 @@
       <c r="Y3" s="5"/>
       <c r="Z3" s="5"/>
     </row>
-    <row r="4" spans="1:26" ht="46.5" customHeight="1">
-      <c r="A4" s="7">
+    <row r="4" spans="1:26" s="28" customFormat="1" ht="46.5" customHeight="1">
+      <c r="A4" s="17">
         <v>1</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="28" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="18"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
-      <c r="T4" s="2"/>
-      <c r="U4" s="2"/>
-      <c r="V4" s="2"/>
-      <c r="W4" s="2"/>
-      <c r="X4" s="2"/>
-      <c r="Y4" s="2"/>
-      <c r="Z4" s="2"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
     </row>
     <row r="5" spans="1:26" ht="27" customHeight="1">
-      <c r="A5" s="28">
+      <c r="A5" s="26">
         <v>2</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="22" t="s">
+      <c r="E5" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="29"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
@@ -846,14 +829,14 @@
       <c r="Z5" s="2"/>
     </row>
     <row r="6" spans="1:26" ht="52.5" customHeight="1">
-      <c r="A6" s="28"/>
-      <c r="B6" s="27"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="28"/>
+      <c r="A6" s="26"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
@@ -886,8 +869,8 @@
       <c r="D7" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="22"/>
-      <c r="F7" s="18"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="15"/>
       <c r="G7" s="9"/>
       <c r="H7" s="8"/>
       <c r="I7" s="2"/>
@@ -922,8 +905,8 @@
       <c r="D8" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="22"/>
-      <c r="F8" s="18"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="15"/>
       <c r="G8" s="9"/>
       <c r="H8" s="8"/>
       <c r="I8" s="2"/>
@@ -959,7 +942,7 @@
         <v>25</v>
       </c>
       <c r="E9" s="7"/>
-      <c r="F9" s="18"/>
+      <c r="F9" s="15"/>
       <c r="G9" s="7"/>
       <c r="H9" s="8"/>
       <c r="I9" s="1"/>
@@ -995,7 +978,7 @@
         <v>28</v>
       </c>
       <c r="E10" s="7"/>
-      <c r="F10" s="18"/>
+      <c r="F10" s="15"/>
       <c r="G10" s="7"/>
       <c r="H10" s="8"/>
       <c r="I10" s="1"/>
@@ -28638,12 +28621,7 @@
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="H5:H6"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="E4" r:id="rId1"/>
-    <hyperlink ref="B4" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3" display="SIQ.xlsx"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updating the RTM , filling the SRS ID's in the RTM and relating them with CRS & SIQ checking the SRS ID's correctness and consistency
</commit_message>
<xml_diff>
--- a/Managment/Requirments/ACS_RTM.xlsx
+++ b/Managment/Requirments/ACS_RTM.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Air-Conditioner-Screen-Team-4\Managment\Requirments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Air-Conditioner-Screen-Team-4\Managment\Requirments\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>REQUIREMENTS TRACEABILITY MATRIX</t>
   </si>
@@ -83,17 +83,9 @@
     <t>SIQ_5</t>
   </si>
   <si>
-    <t>2.0.3</t>
-  </si>
-  <si>
     <t>SIQ_1
 SIQ_4
 SIQ_20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.0.2
-2.0.4
-</t>
   </si>
   <si>
     <t xml:space="preserve">SIQ_7
@@ -160,12 +152,49 @@
 TC_2.3
 TC_2.4</t>
   </si>
+  <si>
+    <t>Version 2.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Version Number:</t>
+  </si>
+  <si>
+    <t>SRS_4.1.1
+SRS_4.1.2</t>
+  </si>
+  <si>
+    <t>SRS_4.1.3
+SRS_4.1.4
+SRS_4.1.5</t>
+  </si>
+  <si>
+    <t>SRS_2.2.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+SRS_4.1.8
+SRS_4.1.9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SRS_4.1.6
+SRS_4.1.7
+</t>
+  </si>
+  <si>
+    <t>SRS_2.2.1
+SRS_2.2.2
+SRS_2.2.3
+SRS_3.1
+SRS_3.2
+SRS_3.3
+SRS_3.4</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -224,6 +253,13 @@
       <name val="Century Gothic"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -251,7 +287,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -259,12 +295,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -306,16 +351,16 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -342,11 +387,23 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -629,10 +686,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z996"/>
+  <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -676,11 +733,11 @@
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
     </row>
-    <row r="2" spans="1:26" ht="12.75">
-      <c r="A2" s="18" t="s">
+    <row r="2" spans="1:26" ht="14.25">
+      <c r="A2" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="19"/>
+      <c r="B2" s="28"/>
       <c r="C2" s="24" t="s">
         <v>3</v>
       </c>
@@ -708,133 +765,137 @@
       <c r="Y2" s="2"/>
       <c r="Z2" s="2"/>
     </row>
-    <row r="3" spans="1:26" s="6" customFormat="1" ht="38.25">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:26" ht="14.25">
+      <c r="A3" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="29"/>
+      <c r="C3" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="2"/>
+      <c r="Z3" s="2"/>
+    </row>
+    <row r="4" spans="1:26" s="6" customFormat="1" ht="38.25">
+      <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B4" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E4" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="5"/>
-      <c r="R3" s="5"/>
-      <c r="S3" s="5"/>
-      <c r="T3" s="5"/>
-      <c r="U3" s="5"/>
-      <c r="V3" s="5"/>
-      <c r="W3" s="5"/>
-      <c r="X3" s="5"/>
-      <c r="Y3" s="5"/>
-      <c r="Z3" s="5"/>
-    </row>
-    <row r="4" spans="1:26" s="28" customFormat="1" ht="46.5" customHeight="1">
-      <c r="A4" s="17">
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5"/>
+      <c r="S4" s="5"/>
+      <c r="T4" s="5"/>
+      <c r="U4" s="5"/>
+      <c r="V4" s="5"/>
+      <c r="W4" s="5"/>
+      <c r="X4" s="5"/>
+      <c r="Y4" s="5"/>
+      <c r="Z4" s="5"/>
+    </row>
+    <row r="5" spans="1:26" s="18" customFormat="1" ht="46.5" customHeight="1">
+      <c r="A5" s="16">
         <v>1</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B5" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="28" t="s">
+      <c r="C5" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="3"/>
-      <c r="R4" s="3"/>
-      <c r="S4" s="3"/>
-      <c r="T4" s="3"/>
-      <c r="U4" s="3"/>
-      <c r="V4" s="3"/>
-      <c r="W4" s="3"/>
-      <c r="X4" s="3"/>
-      <c r="Y4" s="3"/>
-      <c r="Z4" s="3"/>
-    </row>
-    <row r="5" spans="1:26" ht="27" customHeight="1">
-      <c r="A5" s="26">
+      <c r="D5" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="30"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3"/>
+      <c r="X5" s="3"/>
+      <c r="Y5" s="3"/>
+      <c r="Z5" s="3"/>
+    </row>
+    <row r="6" spans="1:26" ht="27" customHeight="1">
+      <c r="A6" s="26">
         <v>2</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="B6" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C6" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="20" t="s">
-        <v>27</v>
+      <c r="D6" s="20" t="s">
+        <v>25</v>
       </c>
-      <c r="E5" s="20" t="s">
-        <v>21</v>
+      <c r="E6" s="20" t="s">
+        <v>35</v>
       </c>
-      <c r="F5" s="27"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="2"/>
-      <c r="R5" s="2"/>
-      <c r="S5" s="2"/>
-      <c r="T5" s="2"/>
-      <c r="U5" s="2"/>
-      <c r="V5" s="2"/>
-      <c r="W5" s="2"/>
-      <c r="X5" s="2"/>
-      <c r="Y5" s="2"/>
-      <c r="Z5" s="2"/>
-    </row>
-    <row r="6" spans="1:26" ht="52.5" customHeight="1">
-      <c r="A6" s="26"/>
-      <c r="B6" s="25"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="27"/>
+      <c r="F6" s="31"/>
       <c r="G6" s="26"/>
       <c r="H6" s="26"/>
       <c r="I6" s="2"/>
@@ -856,23 +917,15 @@
       <c r="Y6" s="2"/>
       <c r="Z6" s="2"/>
     </row>
-    <row r="7" spans="1:26" ht="69.75" customHeight="1">
-      <c r="A7" s="9">
-        <v>3</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>26</v>
-      </c>
+    <row r="7" spans="1:26" ht="52.5" customHeight="1">
+      <c r="A7" s="26"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="20"/>
       <c r="E7" s="20"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="8"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
@@ -892,21 +945,23 @@
       <c r="Y7" s="2"/>
       <c r="Z7" s="2"/>
     </row>
-    <row r="8" spans="1:26" ht="153.75" customHeight="1">
+    <row r="8" spans="1:26" ht="69.75" customHeight="1">
       <c r="A8" s="9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="12" t="s">
-        <v>30</v>
+      <c r="E8" s="17" t="s">
+        <v>34</v>
       </c>
-      <c r="E8" s="20"/>
-      <c r="F8" s="15"/>
+      <c r="F8" s="30"/>
       <c r="G8" s="9"/>
       <c r="H8" s="8"/>
       <c r="I8" s="2"/>
@@ -928,24 +983,26 @@
       <c r="Y8" s="2"/>
       <c r="Z8" s="2"/>
     </row>
-    <row r="9" spans="1:26" ht="40.5">
-      <c r="A9" s="7">
-        <v>5</v>
+    <row r="9" spans="1:26" ht="80.25" customHeight="1">
+      <c r="A9" s="9">
+        <v>4</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
-      <c r="C9" s="11" t="s">
-        <v>18</v>
+      <c r="C9" s="12" t="s">
+        <v>22</v>
       </c>
-      <c r="D9" s="10" t="s">
-        <v>25</v>
+      <c r="D9" s="12" t="s">
+        <v>28</v>
       </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="7"/>
+      <c r="E9" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="30"/>
+      <c r="G9" s="9"/>
       <c r="H9" s="8"/>
-      <c r="I9" s="1"/>
+      <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
@@ -964,21 +1021,23 @@
       <c r="Y9" s="2"/>
       <c r="Z9" s="2"/>
     </row>
-    <row r="10" spans="1:26" ht="78" customHeight="1">
+    <row r="10" spans="1:26" ht="44.25" customHeight="1">
       <c r="A10" s="7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="10" t="s">
-        <v>28</v>
+      <c r="E10" s="17" t="s">
+        <v>33</v>
       </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="15"/>
+      <c r="F10" s="30"/>
       <c r="G10" s="7"/>
       <c r="H10" s="8"/>
       <c r="I10" s="1"/>
@@ -1000,12 +1059,23 @@
       <c r="Y10" s="2"/>
       <c r="Z10" s="2"/>
     </row>
-    <row r="11" spans="1:26" ht="13.5">
-      <c r="A11" s="7"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="10"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
+    <row r="11" spans="1:26" ht="78" customHeight="1">
+      <c r="A11" s="7">
+        <v>6</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" s="30"/>
       <c r="G11" s="7"/>
       <c r="H11" s="8"/>
       <c r="I11" s="1"/>
@@ -1028,14 +1098,13 @@
       <c r="Z11" s="2"/>
     </row>
     <row r="12" spans="1:26" ht="13.5">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
+      <c r="A12" s="7"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="10"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="8"/>
       <c r="I12" s="1"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
@@ -1643,16 +1712,16 @@
       <c r="Y33" s="2"/>
       <c r="Z33" s="2"/>
     </row>
-    <row r="34" spans="1:26" ht="12.75">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
+    <row r="34" spans="1:26" ht="13.5">
+      <c r="A34" s="3"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="1"/>
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
       <c r="L34" s="2"/>
@@ -28607,19 +28676,49 @@
       <c r="Y996" s="2"/>
       <c r="Z996" s="2"/>
     </row>
+    <row r="997" spans="1:26" ht="12.75">
+      <c r="A997" s="2"/>
+      <c r="B997" s="2"/>
+      <c r="C997" s="2"/>
+      <c r="D997" s="2"/>
+      <c r="E997" s="2"/>
+      <c r="F997" s="2"/>
+      <c r="G997" s="2"/>
+      <c r="H997" s="2"/>
+      <c r="I997" s="2"/>
+      <c r="J997" s="2"/>
+      <c r="K997" s="2"/>
+      <c r="L997" s="2"/>
+      <c r="M997" s="2"/>
+      <c r="N997" s="2"/>
+      <c r="O997" s="2"/>
+      <c r="P997" s="2"/>
+      <c r="Q997" s="2"/>
+      <c r="R997" s="2"/>
+      <c r="S997" s="2"/>
+      <c r="T997" s="2"/>
+      <c r="U997" s="2"/>
+      <c r="V997" s="2"/>
+      <c r="W997" s="2"/>
+      <c r="X997" s="2"/>
+      <c r="Y997" s="2"/>
+      <c r="Z997" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="13">
     <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="C6:C7"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="C2:H2"/>
-    <mergeCell ref="E5:E8"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="D6:D7"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="E6:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>